<commit_message>
changed service endpoints order
</commit_message>
<xml_diff>
--- a/Documents/PayrollRestServicesEndpoints.xlsx
+++ b/Documents/PayrollRestServicesEndpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\PayrollEngine\Repos\PayrollEngine\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EFF7D2-6E49-447B-AD3C-F42F0FEBB7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21965E4-19A4-4D68-BE58-EF52E8B34925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="622">
   <si>
     <t>Tenant</t>
   </si>
@@ -1977,9 +1977,6 @@
   </si>
   <si>
     <t>Payroll Engine - REST Service Endpoints</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        </t>
   </si>
   <si>
     <t>an: attribute name</t>
@@ -3169,8 +3166,8 @@
   <dimension ref="B1:K185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="7" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3215,7 +3212,7 @@
     </row>
     <row r="5" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -3452,7 +3449,7 @@
         <v>597</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>183</v>
@@ -3524,7 +3521,7 @@
         <v>172</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E19" s="49" t="s">
         <v>183</v>
@@ -3740,7 +3737,7 @@
         <v>173</v>
       </c>
       <c r="D29" s="57" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E29" s="58" t="s">
         <v>183</v>
@@ -3760,20 +3757,20 @@
     </row>
     <row r="30" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="22" t="s">
-        <v>616</v>
+        <v>186</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>481</v>
+        <v>184</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="24" t="s">
-        <v>269</v>
+        <v>327</v>
       </c>
       <c r="F30" s="43" t="s">
-        <v>482</v>
+        <v>326</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="H30" s="27"/>
       <c r="I30" s="26"/>
@@ -3782,223 +3779,249 @@
     </row>
     <row r="31" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="29" t="s">
-        <v>479</v>
+        <v>186</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>484</v>
+        <v>185</v>
       </c>
       <c r="D31" s="30"/>
       <c r="E31" s="31" t="s">
-        <v>411</v>
+        <v>186</v>
       </c>
       <c r="F31" s="44" t="s">
-        <v>485</v>
+        <v>187</v>
       </c>
       <c r="G31" s="33"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="33"/>
+      <c r="H31" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>474</v>
+      </c>
       <c r="J31" s="5"/>
       <c r="K31" s="9"/>
     </row>
     <row r="32" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="29" t="s">
-        <v>479</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>486</v>
-      </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>487</v>
-      </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="33"/>
+      <c r="B32" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>538</v>
+      </c>
+      <c r="D32" s="57" t="s">
+        <v>616</v>
+      </c>
+      <c r="E32" s="58" t="s">
+        <v>183</v>
+      </c>
+      <c r="F32" s="59" t="s">
+        <v>539</v>
+      </c>
+      <c r="G32" s="60" t="s">
+        <v>540</v>
+      </c>
+      <c r="H32" s="61"/>
+      <c r="I32" s="62" t="s">
+        <v>541</v>
+      </c>
       <c r="J32" s="5"/>
       <c r="K32" s="9"/>
     </row>
     <row r="33" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="29" t="s">
-        <v>479</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>488</v>
-      </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31" t="s">
-        <v>451</v>
-      </c>
-      <c r="F33" s="44" t="s">
-        <v>489</v>
-      </c>
-      <c r="G33" s="33"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="33"/>
+      <c r="B33" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>465</v>
+      </c>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24" t="s">
+        <v>464</v>
+      </c>
+      <c r="F33" s="43" t="s">
+        <v>467</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>469</v>
+      </c>
+      <c r="H33" s="27"/>
+      <c r="I33" s="26"/>
       <c r="J33" s="5"/>
       <c r="K33" s="9"/>
     </row>
     <row r="34" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="29" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>490</v>
+        <v>466</v>
       </c>
       <c r="D34" s="30"/>
       <c r="E34" s="31" t="s">
-        <v>452</v>
+        <v>463</v>
       </c>
       <c r="F34" s="44" t="s">
-        <v>491</v>
+        <v>468</v>
       </c>
       <c r="G34" s="33"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="33"/>
+      <c r="H34" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="I34" s="33" t="s">
+        <v>471</v>
+      </c>
       <c r="J34" s="5"/>
       <c r="K34" s="9"/>
     </row>
     <row r="35" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="29" t="s">
-        <v>479</v>
-      </c>
-      <c r="C35" s="30" t="s">
-        <v>492</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>270</v>
-      </c>
-      <c r="F35" s="44" t="s">
-        <v>493</v>
-      </c>
-      <c r="G35" s="33"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="33"/>
+      <c r="B35" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>542</v>
+      </c>
+      <c r="D35" s="57" t="s">
+        <v>616</v>
+      </c>
+      <c r="E35" s="58" t="s">
+        <v>183</v>
+      </c>
+      <c r="F35" s="59" t="s">
+        <v>543</v>
+      </c>
+      <c r="G35" s="60" t="s">
+        <v>544</v>
+      </c>
+      <c r="H35" s="61"/>
+      <c r="I35" s="62" t="s">
+        <v>545</v>
+      </c>
       <c r="J35" s="5"/>
       <c r="K35" s="9"/>
     </row>
     <row r="36" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="29" t="s">
-        <v>479</v>
-      </c>
-      <c r="C36" s="30" t="s">
-        <v>494</v>
-      </c>
-      <c r="D36" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F36" s="44" t="s">
-        <v>495</v>
-      </c>
-      <c r="G36" s="33"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="33"/>
+      <c r="B36" s="22" t="s">
+        <v>510</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>512</v>
+      </c>
+      <c r="D36" s="23"/>
+      <c r="E36" s="24" t="s">
+        <v>511</v>
+      </c>
+      <c r="F36" s="43" t="s">
+        <v>513</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>514</v>
+      </c>
+      <c r="H36" s="27"/>
+      <c r="I36" s="26"/>
       <c r="J36" s="5"/>
       <c r="K36" s="9"/>
     </row>
     <row r="37" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="36" t="s">
-        <v>479</v>
-      </c>
-      <c r="C37" s="37" t="s">
-        <v>496</v>
-      </c>
-      <c r="D37" s="37"/>
-      <c r="E37" s="38" t="s">
-        <v>419</v>
-      </c>
-      <c r="F37" s="45" t="s">
-        <v>497</v>
-      </c>
-      <c r="G37" s="40"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="40"/>
+      <c r="B37" s="29" t="s">
+        <v>510</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>515</v>
+      </c>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31" t="s">
+        <v>510</v>
+      </c>
+      <c r="F37" s="44" t="s">
+        <v>516</v>
+      </c>
+      <c r="G37" s="33"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="33" t="s">
+        <v>517</v>
+      </c>
       <c r="J37" s="5"/>
       <c r="K37" s="9"/>
     </row>
     <row r="38" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="22" t="s">
-        <v>480</v>
-      </c>
-      <c r="C38" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="F38" s="43" t="s">
-        <v>267</v>
-      </c>
-      <c r="G38" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="H38" s="27"/>
-      <c r="I38" s="26"/>
+      <c r="B38" s="29" t="s">
+        <v>510</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>562</v>
+      </c>
+      <c r="D38" s="30"/>
+      <c r="E38" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="F38" s="44" t="s">
+        <v>558</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>560</v>
+      </c>
+      <c r="H38" s="34"/>
+      <c r="I38" s="33"/>
       <c r="J38" s="5"/>
       <c r="K38" s="9"/>
     </row>
     <row r="39" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="29" t="s">
-        <v>480</v>
-      </c>
-      <c r="C39" s="30" t="s">
-        <v>410</v>
-      </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31" t="s">
-        <v>411</v>
-      </c>
-      <c r="F39" s="44" t="s">
-        <v>412</v>
-      </c>
-      <c r="G39" s="33"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="33"/>
+      <c r="B39" s="36" t="s">
+        <v>510</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>563</v>
+      </c>
+      <c r="D39" s="37"/>
+      <c r="E39" s="38" t="s">
+        <v>556</v>
+      </c>
+      <c r="F39" s="45" t="s">
+        <v>559</v>
+      </c>
+      <c r="G39" s="40"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="40" t="s">
+        <v>561</v>
+      </c>
       <c r="J39" s="5"/>
       <c r="K39" s="9"/>
     </row>
     <row r="40" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="29" t="s">
-        <v>480</v>
-      </c>
-      <c r="C40" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="30"/>
-      <c r="E40" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="F40" s="44" t="s">
-        <v>418</v>
-      </c>
-      <c r="G40" s="33"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="33"/>
+      <c r="B40" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="F40" s="43" t="s">
+        <v>482</v>
+      </c>
+      <c r="G40" s="26" t="s">
+        <v>483</v>
+      </c>
+      <c r="H40" s="27"/>
+      <c r="I40" s="26"/>
       <c r="J40" s="5"/>
       <c r="K40" s="9"/>
     </row>
     <row r="41" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>449</v>
+        <v>484</v>
       </c>
       <c r="D41" s="30"/>
       <c r="E41" s="31" t="s">
-        <v>451</v>
+        <v>411</v>
       </c>
       <c r="F41" s="44" t="s">
-        <v>453</v>
+        <v>485</v>
       </c>
       <c r="G41" s="33"/>
       <c r="H41" s="34"/>
@@ -4008,17 +4031,17 @@
     </row>
     <row r="42" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>450</v>
+        <v>486</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="31" t="s">
-        <v>452</v>
+        <v>45</v>
       </c>
       <c r="F42" s="44" t="s">
-        <v>454</v>
+        <v>487</v>
       </c>
       <c r="G42" s="33"/>
       <c r="H42" s="34"/>
@@ -4028,19 +4051,17 @@
     </row>
     <row r="43" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="30" t="s">
-        <v>36</v>
-      </c>
+        <v>488</v>
+      </c>
+      <c r="D43" s="30"/>
       <c r="E43" s="31" t="s">
-        <v>270</v>
+        <v>451</v>
       </c>
       <c r="F43" s="44" t="s">
-        <v>268</v>
+        <v>489</v>
       </c>
       <c r="G43" s="33"/>
       <c r="H43" s="34"/>
@@ -4050,19 +4071,17 @@
     </row>
     <row r="44" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="30" t="s">
-        <v>36</v>
-      </c>
+        <v>490</v>
+      </c>
+      <c r="D44" s="30"/>
       <c r="E44" s="31" t="s">
-        <v>95</v>
+        <v>452</v>
       </c>
       <c r="F44" s="44" t="s">
-        <v>97</v>
+        <v>491</v>
       </c>
       <c r="G44" s="33"/>
       <c r="H44" s="34"/>
@@ -4071,100 +4090,104 @@
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="36" t="s">
-        <v>480</v>
-      </c>
-      <c r="C45" s="37" t="s">
-        <v>423</v>
-      </c>
-      <c r="D45" s="37"/>
-      <c r="E45" s="38" t="s">
-        <v>419</v>
-      </c>
-      <c r="F45" s="45" t="s">
-        <v>420</v>
-      </c>
-      <c r="G45" s="40"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="40"/>
+      <c r="B45" s="29" t="s">
+        <v>479</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>492</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F45" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="G45" s="33"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="33"/>
       <c r="J45" s="5"/>
       <c r="K45" s="9"/>
     </row>
     <row r="46" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="F46" s="43" t="s">
-        <v>271</v>
-      </c>
-      <c r="G46" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="H46" s="27"/>
-      <c r="I46" s="26"/>
+      <c r="B46" s="29" t="s">
+        <v>479</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>494</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F46" s="44" t="s">
+        <v>495</v>
+      </c>
+      <c r="G46" s="33"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="33"/>
       <c r="J46" s="5"/>
       <c r="K46" s="9"/>
     </row>
     <row r="47" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="30" t="s">
-        <v>413</v>
-      </c>
-      <c r="D47" s="30"/>
-      <c r="E47" s="31" t="s">
-        <v>411</v>
-      </c>
-      <c r="F47" s="44" t="s">
-        <v>414</v>
-      </c>
-      <c r="G47" s="33"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="33"/>
+      <c r="B47" s="36" t="s">
+        <v>479</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>496</v>
+      </c>
+      <c r="D47" s="37"/>
+      <c r="E47" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="F47" s="45" t="s">
+        <v>497</v>
+      </c>
+      <c r="G47" s="40"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="40"/>
       <c r="J47" s="5"/>
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="F48" s="44" t="s">
-        <v>417</v>
-      </c>
-      <c r="G48" s="33"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="33"/>
+      <c r="B48" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="F48" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="H48" s="27"/>
+      <c r="I48" s="26"/>
       <c r="J48" s="5"/>
       <c r="K48" s="9"/>
     </row>
     <row r="49" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="29" t="s">
-        <v>5</v>
+        <v>480</v>
       </c>
       <c r="C49" s="30" t="s">
-        <v>455</v>
+        <v>410</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="31" t="s">
-        <v>451</v>
+        <v>411</v>
       </c>
       <c r="F49" s="44" t="s">
-        <v>457</v>
+        <v>412</v>
       </c>
       <c r="G49" s="33"/>
       <c r="H49" s="34"/>
@@ -4174,17 +4197,17 @@
     </row>
     <row r="50" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="29" t="s">
-        <v>5</v>
+        <v>480</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>456</v>
+        <v>73</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="31" t="s">
-        <v>452</v>
+        <v>45</v>
       </c>
       <c r="F50" s="44" t="s">
-        <v>458</v>
+        <v>418</v>
       </c>
       <c r="G50" s="33"/>
       <c r="H50" s="34"/>
@@ -4194,19 +4217,17 @@
     </row>
     <row r="51" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="29" t="s">
-        <v>5</v>
+        <v>480</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D51" s="30" t="s">
-        <v>36</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="D51" s="30"/>
       <c r="E51" s="31" t="s">
-        <v>270</v>
+        <v>451</v>
       </c>
       <c r="F51" s="44" t="s">
-        <v>272</v>
+        <v>453</v>
       </c>
       <c r="G51" s="33"/>
       <c r="H51" s="34"/>
@@ -4216,19 +4237,17 @@
     </row>
     <row r="52" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="29" t="s">
-        <v>5</v>
+        <v>480</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" s="30" t="s">
-        <v>36</v>
-      </c>
+        <v>450</v>
+      </c>
+      <c r="D52" s="30"/>
       <c r="E52" s="31" t="s">
-        <v>95</v>
+        <v>452</v>
       </c>
       <c r="F52" s="44" t="s">
-        <v>96</v>
+        <v>454</v>
       </c>
       <c r="G52" s="33"/>
       <c r="H52" s="34"/>
@@ -4237,230 +4256,210 @@
       <c r="K52" s="9"/>
     </row>
     <row r="53" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="37" t="s">
-        <v>424</v>
-      </c>
-      <c r="D53" s="37"/>
-      <c r="E53" s="38" t="s">
-        <v>419</v>
-      </c>
-      <c r="F53" s="45" t="s">
-        <v>421</v>
-      </c>
-      <c r="G53" s="40"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="40"/>
+      <c r="B53" s="29" t="s">
+        <v>480</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F53" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="G53" s="33"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="33"/>
       <c r="J53" s="5"/>
       <c r="K53" s="9"/>
     </row>
     <row r="54" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="C54" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="D54" s="23"/>
-      <c r="E54" s="24" t="s">
-        <v>327</v>
-      </c>
-      <c r="F54" s="43" t="s">
-        <v>326</v>
-      </c>
-      <c r="G54" s="26" t="s">
-        <v>472</v>
-      </c>
-      <c r="H54" s="27"/>
-      <c r="I54" s="26"/>
+      <c r="B54" s="29" t="s">
+        <v>480</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F54" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="G54" s="33"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="33"/>
       <c r="J54" s="5"/>
       <c r="K54" s="9"/>
     </row>
     <row r="55" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="C55" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="D55" s="30"/>
-      <c r="E55" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="F55" s="44" t="s">
-        <v>187</v>
-      </c>
-      <c r="G55" s="33"/>
-      <c r="H55" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="I55" s="33" t="s">
-        <v>474</v>
-      </c>
+      <c r="B55" s="36" t="s">
+        <v>480</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>423</v>
+      </c>
+      <c r="D55" s="37"/>
+      <c r="E55" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="F55" s="45" t="s">
+        <v>420</v>
+      </c>
+      <c r="G55" s="40"/>
+      <c r="H55" s="41"/>
+      <c r="I55" s="40"/>
       <c r="J55" s="5"/>
       <c r="K55" s="9"/>
     </row>
     <row r="56" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="56" t="s">
-        <v>186</v>
-      </c>
-      <c r="C56" s="57" t="s">
-        <v>538</v>
-      </c>
-      <c r="D56" s="57" t="s">
-        <v>617</v>
-      </c>
-      <c r="E56" s="58" t="s">
-        <v>183</v>
-      </c>
-      <c r="F56" s="59" t="s">
-        <v>539</v>
-      </c>
-      <c r="G56" s="60" t="s">
-        <v>540</v>
-      </c>
-      <c r="H56" s="61"/>
-      <c r="I56" s="62" t="s">
-        <v>541</v>
-      </c>
+      <c r="B56" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="23"/>
+      <c r="E56" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="F56" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="H56" s="27"/>
+      <c r="I56" s="26"/>
       <c r="J56" s="5"/>
       <c r="K56" s="9"/>
     </row>
     <row r="57" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="22" t="s">
-        <v>463</v>
-      </c>
-      <c r="C57" s="23" t="s">
-        <v>465</v>
-      </c>
-      <c r="D57" s="23"/>
-      <c r="E57" s="24" t="s">
-        <v>464</v>
-      </c>
-      <c r="F57" s="43" t="s">
-        <v>467</v>
-      </c>
-      <c r="G57" s="26" t="s">
-        <v>469</v>
-      </c>
-      <c r="H57" s="27"/>
-      <c r="I57" s="26"/>
+      <c r="B57" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="30" t="s">
+        <v>413</v>
+      </c>
+      <c r="D57" s="30"/>
+      <c r="E57" s="31" t="s">
+        <v>411</v>
+      </c>
+      <c r="F57" s="44" t="s">
+        <v>414</v>
+      </c>
+      <c r="G57" s="33"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="33"/>
       <c r="J57" s="5"/>
       <c r="K57" s="9"/>
     </row>
     <row r="58" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="29" t="s">
-        <v>463</v>
+        <v>5</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>466</v>
+        <v>75</v>
       </c>
       <c r="D58" s="30"/>
       <c r="E58" s="31" t="s">
-        <v>463</v>
+        <v>45</v>
       </c>
       <c r="F58" s="44" t="s">
-        <v>468</v>
+        <v>417</v>
       </c>
       <c r="G58" s="33"/>
-      <c r="H58" s="34" t="s">
-        <v>470</v>
-      </c>
-      <c r="I58" s="33" t="s">
-        <v>471</v>
-      </c>
+      <c r="H58" s="34"/>
+      <c r="I58" s="33"/>
       <c r="J58" s="5"/>
       <c r="K58" s="9"/>
     </row>
     <row r="59" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="56" t="s">
-        <v>463</v>
-      </c>
-      <c r="C59" s="57" t="s">
-        <v>542</v>
-      </c>
-      <c r="D59" s="57" t="s">
-        <v>617</v>
-      </c>
-      <c r="E59" s="58" t="s">
-        <v>183</v>
-      </c>
-      <c r="F59" s="59" t="s">
-        <v>543</v>
-      </c>
-      <c r="G59" s="60" t="s">
-        <v>544</v>
-      </c>
-      <c r="H59" s="61"/>
-      <c r="I59" s="62" t="s">
-        <v>545</v>
-      </c>
+      <c r="B59" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>455</v>
+      </c>
+      <c r="D59" s="30"/>
+      <c r="E59" s="31" t="s">
+        <v>451</v>
+      </c>
+      <c r="F59" s="44" t="s">
+        <v>457</v>
+      </c>
+      <c r="G59" s="33"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="33"/>
       <c r="J59" s="5"/>
       <c r="K59" s="9"/>
     </row>
     <row r="60" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="22" t="s">
-        <v>510</v>
-      </c>
-      <c r="C60" s="23" t="s">
-        <v>512</v>
-      </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="24" t="s">
-        <v>511</v>
-      </c>
-      <c r="F60" s="43" t="s">
-        <v>513</v>
-      </c>
-      <c r="G60" s="26" t="s">
-        <v>514</v>
-      </c>
-      <c r="H60" s="27"/>
-      <c r="I60" s="26"/>
+      <c r="B60" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>456</v>
+      </c>
+      <c r="D60" s="30"/>
+      <c r="E60" s="31" t="s">
+        <v>452</v>
+      </c>
+      <c r="F60" s="44" t="s">
+        <v>458</v>
+      </c>
+      <c r="G60" s="33"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="33"/>
       <c r="J60" s="5"/>
       <c r="K60" s="9"/>
     </row>
     <row r="61" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="29" t="s">
-        <v>510</v>
+        <v>5</v>
       </c>
       <c r="C61" s="30" t="s">
-        <v>515</v>
-      </c>
-      <c r="D61" s="30"/>
+        <v>93</v>
+      </c>
+      <c r="D61" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="E61" s="31" t="s">
-        <v>510</v>
+        <v>270</v>
       </c>
       <c r="F61" s="44" t="s">
-        <v>516</v>
+        <v>272</v>
       </c>
       <c r="G61" s="33"/>
       <c r="H61" s="34"/>
-      <c r="I61" s="33" t="s">
-        <v>517</v>
-      </c>
+      <c r="I61" s="33"/>
       <c r="J61" s="5"/>
       <c r="K61" s="9"/>
     </row>
     <row r="62" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="29" t="s">
-        <v>510</v>
+        <v>5</v>
       </c>
       <c r="C62" s="30" t="s">
-        <v>562</v>
-      </c>
-      <c r="D62" s="30"/>
+        <v>94</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="E62" s="31" t="s">
-        <v>557</v>
+        <v>95</v>
       </c>
       <c r="F62" s="44" t="s">
-        <v>558</v>
-      </c>
-      <c r="G62" s="35" t="s">
-        <v>560</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G62" s="33"/>
       <c r="H62" s="34"/>
       <c r="I62" s="33"/>
       <c r="J62" s="5"/>
@@ -4468,23 +4467,21 @@
     </row>
     <row r="63" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="36" t="s">
-        <v>510</v>
+        <v>5</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>563</v>
+        <v>424</v>
       </c>
       <c r="D63" s="37"/>
       <c r="E63" s="38" t="s">
-        <v>556</v>
+        <v>419</v>
       </c>
       <c r="F63" s="45" t="s">
-        <v>559</v>
+        <v>421</v>
       </c>
       <c r="G63" s="40"/>
       <c r="H63" s="41"/>
-      <c r="I63" s="40" t="s">
-        <v>561</v>
-      </c>
+      <c r="I63" s="40"/>
       <c r="J63" s="5"/>
       <c r="K63" s="9"/>
     </row>
@@ -4542,7 +4539,7 @@
         <v>174</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E66" s="49" t="s">
         <v>183</v>
@@ -4756,7 +4753,7 @@
         <v>362</v>
       </c>
       <c r="D76" s="30" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E76" s="31" t="s">
         <v>190</v>
@@ -4802,7 +4799,7 @@
         <v>546</v>
       </c>
       <c r="D78" s="48" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E78" s="49" t="s">
         <v>183</v>
@@ -5720,7 +5717,7 @@
         <v>409</v>
       </c>
       <c r="D119" s="48" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E119" s="49" t="s">
         <v>183</v>
@@ -5948,7 +5945,7 @@
         <v>226</v>
       </c>
       <c r="D129" s="48" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E129" s="49" t="s">
         <v>183</v>
@@ -6020,7 +6017,7 @@
         <v>229</v>
       </c>
       <c r="D132" s="48" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E132" s="49" t="s">
         <v>183</v>
@@ -6128,7 +6125,7 @@
         <v>576</v>
       </c>
       <c r="D137" s="30" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E137" s="31" t="s">
         <v>364</v>
@@ -6670,7 +6667,7 @@
         <v>175</v>
       </c>
       <c r="D163" s="57" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E163" s="58" t="s">
         <v>183</v>
@@ -6878,7 +6875,7 @@
         <v>248</v>
       </c>
       <c r="D173" s="30" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E173" s="31" t="s">
         <v>251</v>
@@ -7072,7 +7069,7 @@
         <v>176</v>
       </c>
       <c r="D182" s="69" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E182" s="70" t="s">
         <v>183</v>
@@ -7103,7 +7100,7 @@
     </row>
     <row r="184" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B184" s="79" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C184" s="79"/>
       <c r="D184" s="79"/>

</xml_diff>